<commit_message>
Merge: Master Into Sound
</commit_message>
<xml_diff>
--- a/작업 진척 상황.xlsx
+++ b/작업 진척 상황.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WA-LZenos\WA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D3F185-B5A8-4963-893C-1D961F23619B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB96BD2-5BB9-4B77-BFAF-C289F11AC0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D671856-B11B-4C71-AF4F-7DDCD5945FD1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
   <si>
     <t>작업 목록</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -212,10 +212,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>최적화, 모델 적용 필요</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>모델 적용 필요</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -264,10 +260,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>버그 수정 중</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>매니저: 게임 저장 및 불러오기</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -352,11 +344,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>추후 추가 가능, 효과 기획 필요</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>추가 모델 적용 필요, 버그 수정 필요</t>
+    <t>나레이션 녹음 필요</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>추후 추가 가능</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -515,19 +507,19 @@
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -816,7 +808,7 @@
                   <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -831,28 +823,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.7</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1</c:v>
@@ -870,16 +862,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>0.5</c:v>
@@ -888,10 +880,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>0</c:v>
@@ -906,16 +898,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>1</c:v>
@@ -927,40 +919,40 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.75</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.8</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.5</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.2</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="54">
                   <c:v>0</c:v>
@@ -984,7 +976,7 @@
                   <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.25</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>0.5</c:v>
@@ -993,10 +985,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="66">
                   <c:v>0</c:v>
@@ -2071,8 +2063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4322051-15F8-4CC9-8A74-B659B4FA1729}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2111,12 +2103,12 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="7">
         <f>SUM(D3:D41) / COUNT(D3:D41)</f>
-        <v>0.46923076923076923</v>
+        <v>0.77435897435897438</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -2126,7 +2118,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="7"/>
       <c r="C4" t="s">
         <v>2</v>
@@ -2139,7 +2131,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="7"/>
       <c r="C5" t="s">
         <v>3</v>
@@ -2152,7 +2144,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="7"/>
       <c r="C6" t="s">
         <v>4</v>
@@ -2161,11 +2153,11 @@
         <v>0.9</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="7"/>
       <c r="C7" t="s">
         <v>5</v>
@@ -2178,20 +2170,17 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="7"/>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="7"/>
       <c r="C9" t="s">
         <v>7</v>
@@ -2201,7 +2190,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="7"/>
       <c r="C10" t="s">
         <v>32</v>
@@ -2211,7 +2200,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="7"/>
       <c r="C11" t="s">
         <v>33</v>
@@ -2221,106 +2210,97 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="7"/>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="7"/>
       <c r="C13" t="s">
         <v>34</v>
       </c>
       <c r="D13" s="1">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="7"/>
       <c r="C14" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E14" t="s">
-        <v>80</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="7"/>
       <c r="C15" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="7"/>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="7"/>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="7"/>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="7"/>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E19" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="7"/>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="7"/>
       <c r="C21" t="s">
         <v>9</v>
@@ -2330,7 +2310,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="7"/>
       <c r="C22" t="s">
         <v>14</v>
@@ -2340,7 +2320,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="7"/>
       <c r="C23" t="s">
         <v>8</v>
@@ -2350,7 +2330,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="7"/>
       <c r="C24" t="s">
         <v>16</v>
@@ -2360,7 +2340,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="7"/>
       <c r="C25" t="s">
         <v>17</v>
@@ -2370,172 +2350,178 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="7"/>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="7"/>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="7"/>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="10"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="7"/>
       <c r="C29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D29" s="1">
-        <v>0</v>
+        <v>0.8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="7"/>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" s="1">
         <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="7"/>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="7"/>
       <c r="C32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D32" s="1">
-        <v>0</v>
+        <v>0.8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="10"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="7"/>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D33" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="10"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="7"/>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="7"/>
       <c r="C35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="10"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="7"/>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="10"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="7"/>
       <c r="C37" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="10"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="7"/>
       <c r="C38" t="s">
         <v>10</v>
       </c>
       <c r="D38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="7"/>
       <c r="C39" t="s">
         <v>15</v>
       </c>
       <c r="D39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="7"/>
       <c r="C40" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="10"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="7"/>
       <c r="C41" t="s">
         <v>12</v>
       </c>
       <c r="D41" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="8">
-        <f>SUM(D42:D51) / COUNT(D42:D51)</f>
-        <v>0.69499999999999995</v>
+      <c r="B42" s="12">
+        <f>SUM(D42:D59) / COUNT(D42:D59)</f>
+        <v>0.77222222222222214</v>
       </c>
       <c r="C42" t="s">
         <v>27</v>
@@ -2546,7 +2532,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="11"/>
-      <c r="B43" s="8"/>
+      <c r="B43" s="12"/>
       <c r="C43" t="s">
         <v>28</v>
       </c>
@@ -2556,7 +2542,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="11"/>
-      <c r="B44" s="8"/>
+      <c r="B44" s="12"/>
       <c r="C44" t="s">
         <v>31</v>
       </c>
@@ -2566,105 +2552,105 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="11"/>
-      <c r="B45" s="8"/>
+      <c r="B45" s="12"/>
       <c r="C45" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D45" s="1">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="11"/>
-      <c r="B46" s="8"/>
+      <c r="B46" s="12"/>
       <c r="C46" t="s">
         <v>29</v>
       </c>
       <c r="D46" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="11"/>
-      <c r="B47" s="8"/>
+      <c r="B47" s="12"/>
       <c r="C47" t="s">
         <v>30</v>
       </c>
       <c r="D47" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="11"/>
-      <c r="B48" s="8"/>
+      <c r="B48" s="12"/>
       <c r="C48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D48" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="11"/>
-      <c r="B49" s="8"/>
+      <c r="B49" s="12"/>
       <c r="C49" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D49" s="1">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="11"/>
-      <c r="B50" s="8"/>
+      <c r="B50" s="12"/>
       <c r="C50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D50" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="11"/>
-      <c r="B51" s="8"/>
+      <c r="B51" s="12"/>
       <c r="C51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D51" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="11"/>
-      <c r="B52" s="8"/>
+      <c r="B52" s="12"/>
       <c r="C52" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D52" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="11"/>
-      <c r="B53" s="8"/>
+      <c r="B53" s="12"/>
       <c r="C53" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D53" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="11"/>
-      <c r="B54" s="8"/>
+      <c r="B54" s="12"/>
       <c r="C54" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D54" s="1">
         <v>0.7</v>
@@ -2672,29 +2658,29 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="11"/>
-      <c r="B55" s="8"/>
+      <c r="B55" s="12"/>
       <c r="C55" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D55" s="1">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="11"/>
-      <c r="B56" s="8"/>
+      <c r="B56" s="12"/>
       <c r="C56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D56" s="1">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="11"/>
-      <c r="B57" s="8"/>
+      <c r="B57" s="12"/>
       <c r="C57" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D57" s="1">
         <v>0</v>
@@ -2702,9 +2688,9 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="11"/>
-      <c r="B58" s="8"/>
+      <c r="B58" s="12"/>
       <c r="C58" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D58" s="1">
         <v>0</v>
@@ -2712,21 +2698,21 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="11"/>
-      <c r="B59" s="8"/>
+      <c r="B59" s="12"/>
       <c r="C59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D59" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="12" t="s">
+      <c r="A60" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B60" s="9">
+      <c r="B60" s="8">
         <f>SUM(D60:D70) / COUNT(D60:D70)</f>
-        <v>0.31363636363636366</v>
+        <v>0.5</v>
       </c>
       <c r="C60" t="s">
         <v>37</v>
@@ -2736,8 +2722,8 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="12"/>
-      <c r="B61" s="9"/>
+      <c r="A61" s="10"/>
+      <c r="B61" s="8"/>
       <c r="C61" t="s">
         <v>38</v>
       </c>
@@ -2746,18 +2732,18 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="12"/>
-      <c r="B62" s="9"/>
+      <c r="A62" s="10"/>
+      <c r="B62" s="8"/>
       <c r="C62" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D62" s="1">
         <v>0.7</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="12"/>
-      <c r="B63" s="9"/>
+      <c r="A63" s="10"/>
+      <c r="B63" s="8"/>
       <c r="C63" t="s">
         <v>39</v>
       </c>
@@ -2766,18 +2752,18 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="12"/>
-      <c r="B64" s="9"/>
+      <c r="A64" s="10"/>
+      <c r="B64" s="8"/>
       <c r="C64" t="s">
         <v>40</v>
       </c>
       <c r="D64" s="1">
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="12"/>
-      <c r="B65" s="9"/>
+      <c r="A65" s="10"/>
+      <c r="B65" s="8"/>
       <c r="C65" t="s">
         <v>41</v>
       </c>
@@ -2786,38 +2772,38 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="12"/>
-      <c r="B66" s="9"/>
+      <c r="A66" s="10"/>
+      <c r="B66" s="8"/>
       <c r="C66" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D66" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="12"/>
-      <c r="B67" s="9"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="8"/>
       <c r="C67" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="12"/>
-      <c r="B68" s="9"/>
+      <c r="A68" s="10"/>
+      <c r="B68" s="8"/>
       <c r="C68" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D68" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="12"/>
-      <c r="B69" s="9"/>
+      <c r="A69" s="10"/>
+      <c r="B69" s="8"/>
       <c r="C69" t="s">
         <v>42</v>
       </c>
@@ -2826,8 +2812,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="12"/>
-      <c r="B70" s="9"/>
+      <c r="A70" s="10"/>
+      <c r="B70" s="8"/>
       <c r="C70" t="s">
         <v>43</v>
       </c>
@@ -2841,7 +2827,7 @@
       </c>
       <c r="B71" s="4">
         <f>SUM(B3:B70) / 3</f>
-        <v>0.49262237762237765</v>
+        <v>0.68219373219373214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>